<commit_message>
Cleaned file from old records
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,55 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\groos\Documents\GitHub\BasketBot\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134383CB-6E5F-49CF-9CF0-B889F163B936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25620" yWindow="2580" windowWidth="12900" windowHeight="10575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="25620" yWindow="2580" windowWidth="12900" windowHeight="10575" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="4">
-  <si>
-    <t>ср.знач</t>
-  </si>
-  <si>
-    <t>макс</t>
-  </si>
-  <si>
-    <t>мин</t>
-  </si>
-  <si>
-    <t>Score:</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -83,22 +61,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -364,266 +401,344 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B30" sqref="A30:B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>870</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>330</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>ср.знач</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>макс</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>мин</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>476</v>
       </c>
       <c r="D4" s="1">
         <f>AVERAGE(B:B)</f>
-        <v>294.10344827586209</v>
+        <v/>
       </c>
       <c r="E4" s="1">
         <f>MAX(B:B)</f>
-        <v>889</v>
+        <v/>
       </c>
       <c r="F4" s="1">
         <f>MIN(B:B)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6">
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8">
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9">
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>489</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10">
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>284</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11">
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>377</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12">
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13">
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14">
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
         <v>228</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15">
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
         <v>456</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16">
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
         <v>452</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17">
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
         <v>191</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18">
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
         <v>264</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19">
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
         <v>240</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20">
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21">
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22">
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
         <v>252</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23">
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24">
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
         <v>405</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25">
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
         <v>289</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26">
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27">
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
         <v>296</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28">
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
         <v>889</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29">
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
         <v>452</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved version Recalculating a function: - changed initial velocity - gravitational acceleration changed + main function + new comments
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="25620" yWindow="2580" windowWidth="12900" windowHeight="10575" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="25560" yWindow="3420" windowWidth="12900" windowHeight="10575" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
@@ -406,10 +406,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B30" sqref="A30:B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -445,17 +445,17 @@
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>ср.знач</t>
+          <t>Avg.val</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>макс</t>
+          <t>MAX</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>мин</t>
+          <t>MIN</t>
         </is>
       </c>
     </row>
@@ -739,6 +739,1076 @@
       </c>
       <c r="B30" t="n">
         <v>192</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
File BasketBot is for simple launch. BasketBot_v2 is for advanced launch (data collect and replay)
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -406,7 +406,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F137"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -1811,6 +1811,36 @@
         <v>314</v>
       </c>
     </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>536</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes: - Modified coefficient - BasketBot_v2 is working now properly as well as BasketBot - Added new image with score identificator (pink) - Other small changes
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -406,7 +406,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F140"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -1841,6 +1841,26 @@
         <v>536</v>
       </c>
     </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Score:</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>